<commit_message>
Update US trends for wood pulp production.
</commit_message>
<xml_diff>
--- a/input/activity/Wood_Pulp_Consumption.xlsx
+++ b/input/activity/Wood_Pulp_Consumption.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="9320" yWindow="80" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Wood Pulp Cons" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -18,40 +18,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>April</author>
-  </authors>
-  <commentList>
-    <comment ref="DJ137" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-          </rPr>
-          <t>April:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">
-Data source change</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="152">
   <si>
     <t>Consumption (Wood Pulp in tons)</t>
   </si>
@@ -499,12 +467,24 @@
   <si>
     <t>As used in Smith et al. 201`1</t>
   </si>
+  <si>
+    <t>1910/2000</t>
+  </si>
+  <si>
+    <t>1920/2000</t>
+  </si>
+  <si>
+    <t>1900/2000</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <name val="Times"/>
@@ -527,17 +507,6 @@
     <font>
       <sz val="10"/>
       <name val="Times"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
     </font>
     <font>
       <u/>
@@ -590,17 +559,39 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -621,18 +612,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="30">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_TotalConsumptionCoal (ktoe)" xfId="1"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -968,17 +993,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor indexed="50"/>
   </sheetPr>
-  <dimension ref="A1:FE151"/>
+  <dimension ref="A1:FI151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="DE112" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="ES4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B148" sqref="B148"/>
+      <selection pane="bottomRight" activeCell="FG4" sqref="FG4:FG143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -1002,16 +1027,16 @@
     <col min="159" max="159" width="9.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:161">
+    <row r="1" spans="1:165">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:161">
+    <row r="2" spans="1:165">
       <c r="B2"/>
       <c r="C2"/>
     </row>
-    <row r="3" spans="1:161" ht="39">
+    <row r="3" spans="1:165" ht="39">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1495,8 +1520,17 @@
       <c r="FE3" s="4">
         <v>2007</v>
       </c>
+      <c r="FG3" t="s">
+        <v>151</v>
+      </c>
+      <c r="FH3" t="s">
+        <v>149</v>
+      </c>
+      <c r="FI3" t="s">
+        <v>150</v>
+      </c>
     </row>
-    <row r="4" spans="1:161">
+    <row r="4" spans="1:165">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1980,8 +2014,20 @@
       <c r="FE4" s="5">
         <v>0</v>
       </c>
+      <c r="FG4" s="10" t="str">
+        <f>IF($BB4&gt;0,$BB4/$EX4,"")</f>
+        <v/>
+      </c>
+      <c r="FH4" s="10" t="str">
+        <f t="shared" ref="FG4:FH44" si="0">IF($BL4&gt;0,$BL4/$EX4,"")</f>
+        <v/>
+      </c>
+      <c r="FI4" s="10" t="str">
+        <f t="shared" ref="FI4:FI44" si="1">IF($BV4&gt;0,$BV4/$EX4,"")</f>
+        <v/>
+      </c>
     </row>
-    <row r="5" spans="1:161">
+    <row r="5" spans="1:165">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -2465,8 +2511,20 @@
       <c r="FE5" s="5">
         <v>0</v>
       </c>
+      <c r="FG5" s="10" t="str">
+        <f t="shared" ref="FG5:FG68" si="2">IF($BB5&gt;0,$BB5/$EX5,"")</f>
+        <v/>
+      </c>
+      <c r="FH5" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="FI5" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
-    <row r="6" spans="1:161">
+    <row r="6" spans="1:165">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -2950,8 +3008,20 @@
       <c r="FE6" s="5">
         <v>15000</v>
       </c>
+      <c r="FG6" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH6" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="FI6" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
-    <row r="7" spans="1:161">
+    <row r="7" spans="1:165">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -3435,8 +3505,20 @@
       <c r="FE7" s="5">
         <v>794000</v>
       </c>
+      <c r="FG7" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH7" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="FI7" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
-    <row r="8" spans="1:161">
+    <row r="8" spans="1:165">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -3920,8 +4002,20 @@
       <c r="FE8" s="5">
         <v>0</v>
       </c>
+      <c r="FG8" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH8" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="FI8" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
-    <row r="9" spans="1:161">
+    <row r="9" spans="1:165">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -4405,8 +4499,20 @@
       <c r="FE9" s="5">
         <v>1182000</v>
       </c>
+      <c r="FG9" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH9" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="FI9" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
-    <row r="10" spans="1:161">
+    <row r="10" spans="1:165">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -4890,8 +4996,20 @@
       <c r="FE10" s="5">
         <v>1989000</v>
       </c>
+      <c r="FG10" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH10" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="FI10" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
-    <row r="11" spans="1:161">
+    <row r="11" spans="1:165">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -5375,8 +5493,20 @@
       <c r="FE11" s="5">
         <v>0</v>
       </c>
+      <c r="FG11" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH11" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="FI11" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
-    <row r="12" spans="1:161">
+    <row r="12" spans="1:165">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -5860,8 +5990,20 @@
       <c r="FE12" s="5">
         <v>0</v>
       </c>
+      <c r="FG12" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH12" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="FI12" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
-    <row r="13" spans="1:161">
+    <row r="13" spans="1:165">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -6345,8 +6487,20 @@
       <c r="FE13" s="5">
         <v>47000</v>
       </c>
+      <c r="FG13" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH13" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="FI13" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
-    <row r="14" spans="1:161">
+    <row r="14" spans="1:165">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -6830,8 +6984,20 @@
       <c r="FE14" s="5">
         <v>65900</v>
       </c>
+      <c r="FG14" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH14" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="FI14" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
-    <row r="15" spans="1:161">
+    <row r="15" spans="1:165">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -7315,8 +7481,20 @@
       <c r="FE15" s="5">
         <v>509000</v>
       </c>
+      <c r="FG15" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH15" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="FI15" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
-    <row r="16" spans="1:161">
+    <row r="16" spans="1:165">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -7800,8 +7978,20 @@
       <c r="FE16" s="5">
         <v>20000</v>
       </c>
+      <c r="FG16" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH16" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="FI16" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
-    <row r="17" spans="1:161">
+    <row r="17" spans="1:165">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -8285,8 +8475,20 @@
       <c r="FE17" s="5">
         <v>0</v>
       </c>
+      <c r="FG17" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH17" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="FI17" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
-    <row r="18" spans="1:161">
+    <row r="18" spans="1:165">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -8770,8 +8972,20 @@
       <c r="FE18" s="5">
         <v>0</v>
       </c>
+      <c r="FG18" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH18" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="FI18" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
-    <row r="19" spans="1:161">
+    <row r="19" spans="1:165">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -9255,8 +9469,20 @@
       <c r="FE19" s="5">
         <v>0</v>
       </c>
+      <c r="FG19" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH19" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="FI19" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
-    <row r="20" spans="1:161">
+    <row r="20" spans="1:165">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -9740,8 +9966,20 @@
       <c r="FE20" s="5">
         <v>12083000</v>
       </c>
+      <c r="FG20" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH20" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="FI20" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
-    <row r="21" spans="1:161">
+    <row r="21" spans="1:165">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -10225,8 +10463,20 @@
       <c r="FE21" s="5">
         <v>0</v>
       </c>
+      <c r="FG21" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH21" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="FI21" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
-    <row r="22" spans="1:161">
+    <row r="22" spans="1:165">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -10710,8 +10960,20 @@
       <c r="FE22" s="5">
         <v>135000</v>
       </c>
+      <c r="FG22" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH22" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="FI22" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
-    <row r="23" spans="1:161">
+    <row r="23" spans="1:165">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -11195,8 +11457,20 @@
       <c r="FE23" s="5">
         <v>0</v>
       </c>
+      <c r="FG23" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH23" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="FI23" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
-    <row r="24" spans="1:161">
+    <row r="24" spans="1:165">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -11680,8 +11954,20 @@
       <c r="FE24" s="5">
         <v>0</v>
       </c>
+      <c r="FG24" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH24" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="FI24" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
-    <row r="25" spans="1:161">
+    <row r="25" spans="1:165">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -12165,8 +12451,20 @@
       <c r="FE25" s="5">
         <v>22235000</v>
       </c>
+      <c r="FG25" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH25" s="10">
+        <f t="shared" si="0"/>
+        <v>1.7792927779442615E-2</v>
+      </c>
+      <c r="FI25" s="10">
+        <f t="shared" si="1"/>
+        <v>7.3419238837278994E-2</v>
+      </c>
     </row>
-    <row r="26" spans="1:161">
+    <row r="26" spans="1:165">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -12650,8 +12948,20 @@
       <c r="FE26" s="5">
         <v>4675000</v>
       </c>
+      <c r="FG26" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH26" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="FI26" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
-    <row r="27" spans="1:161">
+    <row r="27" spans="1:165">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -13135,8 +13445,20 @@
       <c r="FE27" s="5">
         <v>6435200</v>
       </c>
+      <c r="FG27" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH27" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="FI27" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
-    <row r="28" spans="1:161">
+    <row r="28" spans="1:165">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -13620,8 +13942,20 @@
       <c r="FE28" s="5">
         <v>203000</v>
       </c>
+      <c r="FG28" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH28" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="FI28" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
-    <row r="29" spans="1:161">
+    <row r="29" spans="1:165">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -14105,8 +14439,20 @@
       <c r="FE29" s="5">
         <v>0</v>
       </c>
+      <c r="FG29" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH29" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="FI29" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
-    <row r="30" spans="1:161">
+    <row r="30" spans="1:165">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -14590,8 +14936,20 @@
       <c r="FE30" s="5">
         <v>0</v>
       </c>
+      <c r="FG30" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH30" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="FI30" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
-    <row r="31" spans="1:161">
+    <row r="31" spans="1:165">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -15075,8 +15433,20 @@
       <c r="FE31" s="5">
         <v>2800</v>
       </c>
+      <c r="FG31" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH31" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="FI31" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
-    <row r="32" spans="1:161">
+    <row r="32" spans="1:165">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -15560,8 +15930,20 @@
       <c r="FE32" s="5">
         <v>0</v>
       </c>
+      <c r="FG32" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH32" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="FI32" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
-    <row r="33" spans="1:161">
+    <row r="33" spans="1:165">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -16045,8 +16427,20 @@
       <c r="FE33" s="5">
         <v>97000</v>
       </c>
+      <c r="FG33" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH33" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="FI33" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
-    <row r="34" spans="1:161">
+    <row r="34" spans="1:165">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -16530,8 +16924,20 @@
       <c r="FE34" s="5">
         <v>0</v>
       </c>
+      <c r="FG34" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH34" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="FI34" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
-    <row r="35" spans="1:161">
+    <row r="35" spans="1:165">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -17015,8 +17421,20 @@
       <c r="FE35" s="5">
         <v>0</v>
       </c>
+      <c r="FG35" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH35" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="FI35" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
-    <row r="36" spans="1:161">
+    <row r="36" spans="1:165">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -17500,8 +17918,20 @@
       <c r="FE36" s="5">
         <v>780000</v>
       </c>
+      <c r="FG36" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH36" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="FI36" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
-    <row r="37" spans="1:161">
+    <row r="37" spans="1:165">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -17985,8 +18415,20 @@
       <c r="FE37" s="5">
         <v>0</v>
       </c>
+      <c r="FG37" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH37" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="FI37" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
-    <row r="38" spans="1:161">
+    <row r="38" spans="1:165">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -18470,8 +18912,20 @@
       <c r="FE38" s="5">
         <v>0</v>
       </c>
+      <c r="FG38" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH38" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="FI38" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
-    <row r="39" spans="1:161">
+    <row r="39" spans="1:165">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -18955,8 +19409,20 @@
       <c r="FE39" s="5">
         <v>2000</v>
       </c>
+      <c r="FG39" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH39" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="FI39" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
-    <row r="40" spans="1:161">
+    <row r="40" spans="1:165">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -19440,8 +19906,20 @@
       <c r="FE40" s="5">
         <v>0</v>
       </c>
+      <c r="FG40" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH40" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="FI40" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
-    <row r="41" spans="1:161">
+    <row r="41" spans="1:165">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -19925,8 +20403,20 @@
       <c r="FE41" s="5">
         <v>0</v>
       </c>
+      <c r="FG41" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH41" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="FI41" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
-    <row r="42" spans="1:161">
+    <row r="42" spans="1:165">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -20410,8 +20900,20 @@
       <c r="FE42" s="5">
         <v>0</v>
       </c>
+      <c r="FG42" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH42" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="FI42" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
-    <row r="43" spans="1:161">
+    <row r="43" spans="1:165">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -20895,8 +21397,20 @@
       <c r="FE43" s="5">
         <v>185200</v>
       </c>
+      <c r="FG43" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH43" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="FI43" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
-    <row r="44" spans="1:161">
+    <row r="44" spans="1:165">
       <c r="A44" t="s">
         <v>44</v>
       </c>
@@ -21380,8 +21894,20 @@
       <c r="FE44" s="5">
         <v>0</v>
       </c>
+      <c r="FG44" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH44" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="FI44" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
-    <row r="45" spans="1:161">
+    <row r="45" spans="1:165">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -21865,8 +22391,20 @@
       <c r="FE45" s="5">
         <v>12856000</v>
       </c>
+      <c r="FG45" s="10">
+        <f t="shared" si="2"/>
+        <v>1.165792322424848E-3</v>
+      </c>
+      <c r="FH45" s="10">
+        <f>IF($BL45&gt;0,$BL45/$EX45,"")</f>
+        <v>1.9235573320009993E-2</v>
+      </c>
+      <c r="FI45" s="10">
+        <f>IF($BV45&gt;0,$BV45/$EX45,"")</f>
+        <v>2.6979765176117911E-2</v>
+      </c>
     </row>
-    <row r="46" spans="1:161">
+    <row r="46" spans="1:165">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -22350,8 +22888,20 @@
       <c r="FE46" s="5">
         <v>2259600</v>
       </c>
+      <c r="FG46" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH46" s="10" t="str">
+        <f t="shared" ref="FG46:FH109" si="3">IF($BL46&gt;0,$BL46/$EX46,"")</f>
+        <v/>
+      </c>
+      <c r="FI46" s="10" t="str">
+        <f t="shared" ref="FI46:FI109" si="4">IF($BV46&gt;0,$BV46/$EX46,"")</f>
+        <v/>
+      </c>
     </row>
-    <row r="47" spans="1:161">
+    <row r="47" spans="1:165">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -22835,8 +23385,20 @@
       <c r="FE47" s="5">
         <v>0</v>
       </c>
+      <c r="FG47" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH47" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI47" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="48" spans="1:161">
+    <row r="48" spans="1:165">
       <c r="A48" t="s">
         <v>48</v>
       </c>
@@ -23320,8 +23882,20 @@
       <c r="FE48" s="5">
         <v>0</v>
       </c>
+      <c r="FG48" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH48" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI48" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="49" spans="1:161">
+    <row r="49" spans="1:165">
       <c r="A49" t="s">
         <v>49</v>
       </c>
@@ -23805,8 +24379,20 @@
       <c r="FE49" s="5">
         <v>0</v>
       </c>
+      <c r="FG49" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH49" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI49" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="50" spans="1:161">
+    <row r="50" spans="1:165">
       <c r="A50" t="s">
         <v>50</v>
       </c>
@@ -24290,8 +24876,20 @@
       <c r="FE50" s="5">
         <v>3001000</v>
       </c>
+      <c r="FG50" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH50" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI50" s="10">
+        <f t="shared" si="4"/>
+        <v>0.18058690744920994</v>
+      </c>
     </row>
-    <row r="51" spans="1:161">
+    <row r="51" spans="1:165">
       <c r="A51" t="s">
         <v>51</v>
       </c>
@@ -24775,8 +25373,20 @@
       <c r="FE51" s="5">
         <v>0</v>
       </c>
+      <c r="FG51" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH51" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI51" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="52" spans="1:161">
+    <row r="52" spans="1:165">
       <c r="A52" t="s">
         <v>52</v>
       </c>
@@ -25260,8 +25870,20 @@
       <c r="FE52" s="5">
         <v>0</v>
       </c>
+      <c r="FG52" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH52" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI52" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="53" spans="1:161">
+    <row r="53" spans="1:165">
       <c r="A53" t="s">
         <v>53</v>
       </c>
@@ -25745,8 +26367,20 @@
       <c r="FE53" s="5">
         <v>0</v>
       </c>
+      <c r="FG53" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH53" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI53" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="54" spans="1:161">
+    <row r="54" spans="1:165">
       <c r="A54" t="s">
         <v>54</v>
       </c>
@@ -26230,8 +26864,20 @@
       <c r="FE54" s="5">
         <v>0</v>
       </c>
+      <c r="FG54" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH54" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI54" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="55" spans="1:161">
+    <row r="55" spans="1:165">
       <c r="A55" t="s">
         <v>55</v>
       </c>
@@ -26715,8 +27361,20 @@
       <c r="FE55" s="5">
         <v>0</v>
       </c>
+      <c r="FG55" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH55" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI55" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="56" spans="1:161">
+    <row r="56" spans="1:165">
       <c r="A56" t="s">
         <v>56</v>
       </c>
@@ -27200,8 +27858,20 @@
       <c r="FE56" s="5">
         <v>7000</v>
       </c>
+      <c r="FG56" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH56" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI56" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="57" spans="1:161">
+    <row r="57" spans="1:165">
       <c r="A57" t="s">
         <v>57</v>
       </c>
@@ -27685,8 +28355,20 @@
       <c r="FE57" s="5">
         <v>0</v>
       </c>
+      <c r="FG57" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH57" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI57" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="58" spans="1:161">
+    <row r="58" spans="1:165">
       <c r="A58" t="s">
         <v>58</v>
       </c>
@@ -28170,8 +28852,20 @@
       <c r="FE58" s="5">
         <v>0</v>
       </c>
+      <c r="FG58" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH58" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI58" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="59" spans="1:161">
+    <row r="59" spans="1:165">
       <c r="A59" t="s">
         <v>59</v>
       </c>
@@ -28655,8 +29349,20 @@
       <c r="FE59" s="5">
         <v>0</v>
       </c>
+      <c r="FG59" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH59" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI59" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="60" spans="1:161">
+    <row r="60" spans="1:165">
       <c r="A60" t="s">
         <v>60</v>
       </c>
@@ -29140,8 +29846,20 @@
       <c r="FE60" s="5">
         <v>2307600</v>
       </c>
+      <c r="FG60" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH60" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI60" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="61" spans="1:161">
+    <row r="61" spans="1:165">
       <c r="A61" t="s">
         <v>61</v>
       </c>
@@ -29625,8 +30343,20 @@
       <c r="FE61" s="5">
         <v>5177000</v>
       </c>
+      <c r="FG61" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH61" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI61" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="62" spans="1:161">
+    <row r="62" spans="1:165">
       <c r="A62" t="s">
         <v>62</v>
       </c>
@@ -30110,8 +30840,20 @@
       <c r="FE62" s="5">
         <v>445000</v>
       </c>
+      <c r="FG62" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH62" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI62" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="63" spans="1:161">
+    <row r="63" spans="1:165">
       <c r="A63" t="s">
         <v>63</v>
       </c>
@@ -30595,8 +31337,20 @@
       <c r="FE63" s="5">
         <v>0</v>
       </c>
+      <c r="FG63" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH63" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI63" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="64" spans="1:161">
+    <row r="64" spans="1:165">
       <c r="A64" t="s">
         <v>64</v>
       </c>
@@ -31080,8 +31834,20 @@
       <c r="FE64" s="5">
         <v>0</v>
       </c>
+      <c r="FG64" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH64" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI64" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="65" spans="1:161">
+    <row r="65" spans="1:165">
       <c r="A65" t="s">
         <v>65</v>
       </c>
@@ -31565,8 +32331,20 @@
       <c r="FE65" s="5">
         <v>0</v>
       </c>
+      <c r="FG65" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH65" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI65" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="66" spans="1:161">
+    <row r="66" spans="1:165">
       <c r="A66" t="s">
         <v>66</v>
       </c>
@@ -32050,8 +32828,20 @@
       <c r="FE66" s="5">
         <v>544000</v>
       </c>
+      <c r="FG66" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH66" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI66" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="67" spans="1:161">
+    <row r="67" spans="1:165">
       <c r="A67" t="s">
         <v>67</v>
       </c>
@@ -32535,8 +33325,20 @@
       <c r="FE67" s="5">
         <v>0</v>
       </c>
+      <c r="FG67" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH67" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI67" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="68" spans="1:161">
+    <row r="68" spans="1:165">
       <c r="A68" t="s">
         <v>68</v>
       </c>
@@ -33020,8 +33822,20 @@
       <c r="FE68" s="5">
         <v>10850000</v>
       </c>
+      <c r="FG68" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="FH68" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI68" s="10">
+        <f t="shared" si="4"/>
+        <v>2.3564582783786162E-2</v>
+      </c>
     </row>
-    <row r="69" spans="1:161">
+    <row r="69" spans="1:165">
       <c r="A69" t="s">
         <v>69</v>
       </c>
@@ -33505,8 +34319,20 @@
       <c r="FE69" s="5">
         <v>0</v>
       </c>
+      <c r="FG69" s="10" t="str">
+        <f t="shared" ref="FG69:FG132" si="5">IF($BB69&gt;0,$BB69/$EX69,"")</f>
+        <v/>
+      </c>
+      <c r="FH69" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI69" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="70" spans="1:161">
+    <row r="70" spans="1:165">
       <c r="A70" t="s">
         <v>70</v>
       </c>
@@ -33990,8 +34816,20 @@
       <c r="FE70" s="5">
         <v>0</v>
       </c>
+      <c r="FG70" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH70" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI70" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="71" spans="1:161">
+    <row r="71" spans="1:165">
       <c r="A71" t="s">
         <v>71</v>
       </c>
@@ -34475,8 +35313,20 @@
       <c r="FE71" s="5">
         <v>86000</v>
       </c>
+      <c r="FG71" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH71" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI71" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="72" spans="1:161">
+    <row r="72" spans="1:165">
       <c r="A72" t="s">
         <v>72</v>
       </c>
@@ -34960,8 +35810,20 @@
       <c r="FE72" s="5">
         <v>418000</v>
       </c>
+      <c r="FG72" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH72" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI72" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="73" spans="1:161">
+    <row r="73" spans="1:165">
       <c r="A73" t="s">
         <v>73</v>
       </c>
@@ -35445,8 +36307,20 @@
       <c r="FE73" s="5">
         <v>56000</v>
       </c>
+      <c r="FG73" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH73" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI73" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="74" spans="1:161">
+    <row r="74" spans="1:165">
       <c r="A74" t="s">
         <v>74</v>
       </c>
@@ -35930,8 +36804,20 @@
       <c r="FE74" s="5">
         <v>0</v>
       </c>
+      <c r="FG74" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH74" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI74" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="75" spans="1:161">
+    <row r="75" spans="1:165">
       <c r="A75" t="s">
         <v>75</v>
       </c>
@@ -36415,8 +37301,20 @@
       <c r="FE75" s="5">
         <v>0</v>
       </c>
+      <c r="FG75" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH75" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI75" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="76" spans="1:161">
+    <row r="76" spans="1:165">
       <c r="A76" t="s">
         <v>76</v>
       </c>
@@ -36900,8 +37798,20 @@
       <c r="FE76" s="5">
         <v>0</v>
       </c>
+      <c r="FG76" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH76" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI76" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="77" spans="1:161">
+    <row r="77" spans="1:165">
       <c r="A77" t="s">
         <v>77</v>
       </c>
@@ -37385,8 +38295,20 @@
       <c r="FE77" s="5">
         <v>0</v>
       </c>
+      <c r="FG77" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH77" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI77" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="78" spans="1:161">
+    <row r="78" spans="1:165">
       <c r="A78" t="s">
         <v>78</v>
       </c>
@@ -37870,8 +38792,20 @@
       <c r="FE78" s="5">
         <v>0</v>
       </c>
+      <c r="FG78" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH78" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI78" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="79" spans="1:161">
+    <row r="79" spans="1:165">
       <c r="A79" t="s">
         <v>79</v>
       </c>
@@ -38355,8 +39289,20 @@
       <c r="FE79" s="5">
         <v>0</v>
       </c>
+      <c r="FG79" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH79" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI79" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="80" spans="1:161">
+    <row r="80" spans="1:165">
       <c r="A80" t="s">
         <v>80</v>
       </c>
@@ -38840,8 +39786,20 @@
       <c r="FE80" s="5">
         <v>0</v>
       </c>
+      <c r="FG80" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH80" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI80" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="81" spans="1:161">
+    <row r="81" spans="1:165">
       <c r="A81" t="s">
         <v>81</v>
       </c>
@@ -39325,8 +40283,20 @@
       <c r="FE81" s="5">
         <v>123000</v>
       </c>
+      <c r="FG81" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH81" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI81" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="82" spans="1:161">
+    <row r="82" spans="1:165">
       <c r="A82" t="s">
         <v>82</v>
       </c>
@@ -39810,8 +40780,20 @@
       <c r="FE82" s="5">
         <v>0</v>
       </c>
+      <c r="FG82" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH82" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI82" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="83" spans="1:161">
+    <row r="83" spans="1:165">
       <c r="A83" t="s">
         <v>83</v>
       </c>
@@ -40295,8 +41277,20 @@
       <c r="FE83" s="5">
         <v>333000</v>
       </c>
+      <c r="FG83" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH83" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI83" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="84" spans="1:161">
+    <row r="84" spans="1:165">
       <c r="A84" t="s">
         <v>84</v>
       </c>
@@ -40780,8 +41774,20 @@
       <c r="FE84" s="5">
         <v>0</v>
       </c>
+      <c r="FG84" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH84" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI84" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="85" spans="1:161">
+    <row r="85" spans="1:165">
       <c r="A85" t="s">
         <v>85</v>
       </c>
@@ -41265,8 +42271,20 @@
       <c r="FE85" s="5">
         <v>0</v>
       </c>
+      <c r="FG85" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH85" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI85" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="86" spans="1:161">
+    <row r="86" spans="1:165">
       <c r="A86" t="s">
         <v>86</v>
       </c>
@@ -41750,8 +42768,20 @@
       <c r="FE86" s="5">
         <v>216000</v>
       </c>
+      <c r="FG86" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH86" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI86" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="87" spans="1:161">
+    <row r="87" spans="1:165">
       <c r="A87" t="s">
         <v>87</v>
       </c>
@@ -42235,8 +43265,20 @@
       <c r="FE87" s="5">
         <v>0</v>
       </c>
+      <c r="FG87" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH87" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI87" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="88" spans="1:161">
+    <row r="88" spans="1:165">
       <c r="A88" t="s">
         <v>88</v>
       </c>
@@ -42720,8 +43762,20 @@
       <c r="FE88" s="5">
         <v>1200</v>
       </c>
+      <c r="FG88" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH88" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI88" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="89" spans="1:161">
+    <row r="89" spans="1:165">
       <c r="A89" t="s">
         <v>89</v>
       </c>
@@ -43205,8 +44259,20 @@
       <c r="FE89" s="5">
         <v>0</v>
       </c>
+      <c r="FG89" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH89" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI89" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="90" spans="1:161">
+    <row r="90" spans="1:165">
       <c r="A90" t="s">
         <v>90</v>
       </c>
@@ -43690,8 +44756,20 @@
       <c r="FE90" s="5">
         <v>0</v>
       </c>
+      <c r="FG90" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH90" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI90" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="91" spans="1:161">
+    <row r="91" spans="1:165">
       <c r="A91" t="s">
         <v>91</v>
       </c>
@@ -44175,8 +45253,20 @@
       <c r="FE91" s="5">
         <v>0</v>
       </c>
+      <c r="FG91" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH91" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI91" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="92" spans="1:161">
+    <row r="92" spans="1:165">
       <c r="A92" t="s">
         <v>92</v>
       </c>
@@ -44660,8 +45750,20 @@
       <c r="FE92" s="5">
         <v>119000</v>
       </c>
+      <c r="FG92" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH92" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI92" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="93" spans="1:161">
+    <row r="93" spans="1:165">
       <c r="A93" t="s">
         <v>93</v>
       </c>
@@ -45145,8 +46247,20 @@
       <c r="FE93" s="5">
         <v>0</v>
       </c>
+      <c r="FG93" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH93" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI93" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="94" spans="1:161">
+    <row r="94" spans="1:165">
       <c r="A94" t="s">
         <v>94</v>
       </c>
@@ -45630,8 +46744,20 @@
       <c r="FE94" s="5">
         <v>23000</v>
       </c>
+      <c r="FG94" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH94" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI94" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="95" spans="1:161">
+    <row r="95" spans="1:165">
       <c r="A95" t="s">
         <v>95</v>
       </c>
@@ -46115,8 +47241,20 @@
       <c r="FE95" s="5">
         <v>2240000</v>
       </c>
+      <c r="FG95" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH95" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI95" s="10">
+        <f t="shared" si="4"/>
+        <v>0.25768321513002362</v>
+      </c>
     </row>
-    <row r="96" spans="1:161" ht="11.25" customHeight="1">
+    <row r="96" spans="1:165" ht="11.25" customHeight="1">
       <c r="A96" t="s">
         <v>96</v>
       </c>
@@ -46600,8 +47738,20 @@
       <c r="FE96" s="5">
         <v>1529000</v>
       </c>
+      <c r="FG96" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH96" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI96" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="97" spans="1:161">
+    <row r="97" spans="1:165">
       <c r="A97" t="s">
         <v>97</v>
       </c>
@@ -47085,8 +48235,20 @@
       <c r="FE97" s="5">
         <v>0</v>
       </c>
+      <c r="FG97" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH97" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI97" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="98" spans="1:161">
+    <row r="98" spans="1:165">
       <c r="A98" t="s">
         <v>98</v>
       </c>
@@ -47570,8 +48732,20 @@
       <c r="FE98" s="5">
         <v>0</v>
       </c>
+      <c r="FG98" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH98" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI98" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="99" spans="1:161">
+    <row r="99" spans="1:165">
       <c r="A99" t="s">
         <v>99</v>
       </c>
@@ -48055,8 +49229,20 @@
       <c r="FE99" s="5">
         <v>0</v>
       </c>
+      <c r="FG99" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH99" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI99" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="100" spans="1:161">
+    <row r="100" spans="1:165">
       <c r="A100" t="s">
         <v>100</v>
       </c>
@@ -48540,8 +49726,20 @@
       <c r="FE100" s="5">
         <v>0</v>
       </c>
+      <c r="FG100" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH100" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI100" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="101" spans="1:161">
+    <row r="101" spans="1:165">
       <c r="A101" t="s">
         <v>101</v>
       </c>
@@ -49025,8 +50223,20 @@
       <c r="FE101" s="5">
         <v>22000</v>
       </c>
+      <c r="FG101" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH101" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI101" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="102" spans="1:161">
+    <row r="102" spans="1:165">
       <c r="A102" t="s">
         <v>102</v>
       </c>
@@ -49510,8 +50720,20 @@
       <c r="FE102" s="5">
         <v>0</v>
       </c>
+      <c r="FG102" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH102" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI102" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="103" spans="1:161">
+    <row r="103" spans="1:165">
       <c r="A103" t="s">
         <v>103</v>
       </c>
@@ -49995,8 +51217,20 @@
       <c r="FE103" s="5">
         <v>0</v>
       </c>
+      <c r="FG103" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH103" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI103" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="104" spans="1:161">
+    <row r="104" spans="1:165">
       <c r="A104" t="s">
         <v>104</v>
       </c>
@@ -50480,8 +51714,20 @@
       <c r="FE104" s="5">
         <v>0</v>
       </c>
+      <c r="FG104" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH104" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI104" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="105" spans="1:161">
+    <row r="105" spans="1:165">
       <c r="A105" t="s">
         <v>105</v>
       </c>
@@ -50965,8 +52211,20 @@
       <c r="FE105" s="5">
         <v>185000</v>
       </c>
+      <c r="FG105" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH105" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI105" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="106" spans="1:161">
+    <row r="106" spans="1:165">
       <c r="A106" t="s">
         <v>106</v>
       </c>
@@ -51450,8 +52708,20 @@
       <c r="FE106" s="5">
         <v>1055782</v>
       </c>
+      <c r="FG106" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH106" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI106" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="107" spans="1:161">
+    <row r="107" spans="1:165">
       <c r="A107" t="s">
         <v>107</v>
       </c>
@@ -51935,8 +53205,20 @@
       <c r="FE107" s="5">
         <v>2065000</v>
       </c>
+      <c r="FG107" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH107" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI107" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="108" spans="1:161">
+    <row r="108" spans="1:165">
       <c r="A108" t="s">
         <v>108</v>
       </c>
@@ -52420,8 +53702,20 @@
       <c r="FE108" s="5">
         <v>0</v>
       </c>
+      <c r="FG108" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH108" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI108" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="109" spans="1:161">
+    <row r="109" spans="1:165">
       <c r="A109" t="s">
         <v>109</v>
       </c>
@@ -52905,8 +54199,20 @@
       <c r="FE109" s="5">
         <v>169000</v>
       </c>
+      <c r="FG109" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH109" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="FI109" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
-    <row r="110" spans="1:161">
+    <row r="110" spans="1:165">
       <c r="A110" t="s">
         <v>110</v>
       </c>
@@ -53390,8 +54696,20 @@
       <c r="FE110" s="5">
         <v>7010000</v>
       </c>
+      <c r="FG110" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH110" s="10" t="str">
+        <f t="shared" ref="FG110:FH143" si="6">IF($BL110&gt;0,$BL110/$EX110,"")</f>
+        <v/>
+      </c>
+      <c r="FI110" s="10" t="str">
+        <f t="shared" ref="FI110:FI143" si="7">IF($BV110&gt;0,$BV110/$EX110,"")</f>
+        <v/>
+      </c>
     </row>
-    <row r="111" spans="1:161">
+    <row r="111" spans="1:165">
       <c r="A111" t="s">
         <v>111</v>
       </c>
@@ -53875,8 +55193,20 @@
       <c r="FE111" s="5">
         <v>0</v>
       </c>
+      <c r="FG111" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH111" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="FI111" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
     </row>
-    <row r="112" spans="1:161">
+    <row r="112" spans="1:165">
       <c r="A112" t="s">
         <v>112</v>
       </c>
@@ -54360,8 +55690,20 @@
       <c r="FE112" s="5">
         <v>0</v>
       </c>
+      <c r="FG112" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH112" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="FI112" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
     </row>
-    <row r="113" spans="1:161">
+    <row r="113" spans="1:165">
       <c r="A113" t="s">
         <v>113</v>
       </c>
@@ -54845,8 +56187,20 @@
       <c r="FE113" s="5">
         <v>0</v>
       </c>
+      <c r="FG113" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH113" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="FI113" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
     </row>
-    <row r="114" spans="1:161">
+    <row r="114" spans="1:165">
       <c r="A114" t="s">
         <v>114</v>
       </c>
@@ -55330,8 +56684,20 @@
       <c r="FE114" s="5">
         <v>0</v>
       </c>
+      <c r="FG114" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH114" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="FI114" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
     </row>
-    <row r="115" spans="1:161">
+    <row r="115" spans="1:165">
       <c r="A115" t="s">
         <v>115</v>
       </c>
@@ -55815,8 +57181,20 @@
       <c r="FE115" s="5">
         <v>664000</v>
       </c>
+      <c r="FG115" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH115" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="FI115" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
     </row>
-    <row r="116" spans="1:161">
+    <row r="116" spans="1:165">
       <c r="A116" t="s">
         <v>116</v>
       </c>
@@ -56300,8 +57678,20 @@
       <c r="FE116" s="5">
         <v>112000</v>
       </c>
+      <c r="FG116" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH116" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="FI116" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
     </row>
-    <row r="117" spans="1:161">
+    <row r="117" spans="1:165">
       <c r="A117" t="s">
         <v>117</v>
       </c>
@@ -56785,8 +58175,20 @@
       <c r="FE117" s="5">
         <v>2310000</v>
       </c>
+      <c r="FG117" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH117" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="FI117" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
     </row>
-    <row r="118" spans="1:161">
+    <row r="118" spans="1:165">
       <c r="A118" t="s">
         <v>118</v>
       </c>
@@ -57270,8 +58672,20 @@
       <c r="FE118" s="5">
         <v>2065235</v>
       </c>
+      <c r="FG118" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH118" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="FI118" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
     </row>
-    <row r="119" spans="1:161">
+    <row r="119" spans="1:165">
       <c r="A119" t="s">
         <v>119</v>
       </c>
@@ -57755,8 +59169,20 @@
       <c r="FE119" s="5">
         <v>2600</v>
       </c>
+      <c r="FG119" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH119" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="FI119" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
     </row>
-    <row r="120" spans="1:161">
+    <row r="120" spans="1:165">
       <c r="A120" t="s">
         <v>120</v>
       </c>
@@ -58240,8 +59666,20 @@
       <c r="FE120" s="5">
         <v>0</v>
       </c>
+      <c r="FG120" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH120" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="FI120" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
     </row>
-    <row r="121" spans="1:161">
+    <row r="121" spans="1:165">
       <c r="A121" t="s">
         <v>121</v>
       </c>
@@ -58725,8 +60163,20 @@
       <c r="FE121" s="5">
         <v>12588000</v>
       </c>
+      <c r="FG121" s="10">
+        <f t="shared" si="5"/>
+        <v>2.7544391511476831E-2</v>
+      </c>
+      <c r="FH121" s="10">
+        <f t="shared" si="6"/>
+        <v>8.1507145950627982E-2</v>
+      </c>
+      <c r="FI121" s="10">
+        <f t="shared" si="7"/>
+        <v>0.11251624079688177</v>
+      </c>
     </row>
-    <row r="122" spans="1:161">
+    <row r="122" spans="1:165">
       <c r="A122" t="s">
         <v>122</v>
       </c>
@@ -59210,8 +60660,20 @@
       <c r="FE122" s="5">
         <v>337000</v>
       </c>
+      <c r="FG122" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH122" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="FI122" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
     </row>
-    <row r="123" spans="1:161">
+    <row r="123" spans="1:165">
       <c r="A123" t="s">
         <v>123</v>
       </c>
@@ -59695,8 +61157,20 @@
       <c r="FE123" s="5">
         <v>0</v>
       </c>
+      <c r="FG123" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH123" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="FI123" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
     </row>
-    <row r="124" spans="1:161">
+    <row r="124" spans="1:165">
       <c r="A124" t="s">
         <v>124</v>
       </c>
@@ -60180,8 +61654,20 @@
       <c r="FE124" s="5">
         <v>0</v>
       </c>
+      <c r="FG124" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH124" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="FI124" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
     </row>
-    <row r="125" spans="1:161">
+    <row r="125" spans="1:165">
       <c r="A125" t="s">
         <v>125</v>
       </c>
@@ -60665,8 +62151,20 @@
       <c r="FE125" s="5">
         <v>0</v>
       </c>
+      <c r="FG125" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH125" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="FI125" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
     </row>
-    <row r="126" spans="1:161">
+    <row r="126" spans="1:165">
       <c r="A126" t="s">
         <v>126</v>
       </c>
@@ -61150,8 +62648,20 @@
       <c r="FE126" s="5">
         <v>56000</v>
       </c>
+      <c r="FG126" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH126" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="FI126" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
     </row>
-    <row r="127" spans="1:161">
+    <row r="127" spans="1:165">
       <c r="A127" t="s">
         <v>127</v>
       </c>
@@ -61635,8 +63145,20 @@
       <c r="FE127" s="5">
         <v>1025000</v>
       </c>
+      <c r="FG127" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH127" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="FI127" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
     </row>
-    <row r="128" spans="1:161">
+    <row r="128" spans="1:165">
       <c r="A128" t="s">
         <v>128</v>
       </c>
@@ -62120,8 +63642,20 @@
       <c r="FE128" s="5">
         <v>0</v>
       </c>
+      <c r="FG128" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH128" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="FI128" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
     </row>
-    <row r="129" spans="1:161">
+    <row r="129" spans="1:165">
       <c r="A129" t="s">
         <v>129</v>
       </c>
@@ -62605,8 +64139,20 @@
       <c r="FE129" s="5">
         <v>0</v>
       </c>
+      <c r="FG129" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH129" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="FI129" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
     </row>
-    <row r="130" spans="1:161">
+    <row r="130" spans="1:165">
       <c r="A130" t="s">
         <v>130</v>
       </c>
@@ -63090,8 +64636,20 @@
       <c r="FE130" s="5">
         <v>0</v>
       </c>
+      <c r="FG130" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH130" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="FI130" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
     </row>
-    <row r="131" spans="1:161">
+    <row r="131" spans="1:165">
       <c r="A131" t="s">
         <v>131</v>
       </c>
@@ -63575,8 +65133,20 @@
       <c r="FE131" s="5">
         <v>75000</v>
       </c>
+      <c r="FG131" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH131" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="FI131" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
     </row>
-    <row r="132" spans="1:161">
+    <row r="132" spans="1:165">
       <c r="A132" t="s">
         <v>132</v>
       </c>
@@ -64060,8 +65630,20 @@
       <c r="FE132" s="5">
         <v>0</v>
       </c>
+      <c r="FG132" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="FH132" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="FI132" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
     </row>
-    <row r="133" spans="1:161">
+    <row r="133" spans="1:165">
       <c r="A133" t="s">
         <v>133</v>
       </c>
@@ -64545,8 +66127,20 @@
       <c r="FE133" s="5">
         <v>0</v>
       </c>
+      <c r="FG133" s="10" t="str">
+        <f t="shared" ref="FG133:FG143" si="8">IF($BB133&gt;0,$BB133/$EX133,"")</f>
+        <v/>
+      </c>
+      <c r="FH133" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="FI133" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
     </row>
-    <row r="134" spans="1:161">
+    <row r="134" spans="1:165">
       <c r="A134" t="s">
         <v>134</v>
       </c>
@@ -65030,8 +66624,20 @@
       <c r="FE134" s="5">
         <v>264000</v>
       </c>
+      <c r="FG134" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="FH134" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="FI134" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
     </row>
-    <row r="135" spans="1:161">
+    <row r="135" spans="1:165">
       <c r="A135" t="s">
         <v>135</v>
       </c>
@@ -65515,8 +67121,20 @@
       <c r="FE135" s="5">
         <v>0</v>
       </c>
+      <c r="FG135" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="FH135" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="FI135" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
     </row>
-    <row r="136" spans="1:161">
+    <row r="136" spans="1:165">
       <c r="A136" t="s">
         <v>136</v>
       </c>
@@ -66000,8 +67618,20 @@
       <c r="FE136" s="5">
         <v>32000</v>
       </c>
+      <c r="FG136" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="FH136" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="FI136" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
     </row>
-    <row r="137" spans="1:161">
+    <row r="137" spans="1:165">
       <c r="A137" t="s">
         <v>137</v>
       </c>
@@ -66132,217 +67762,217 @@
         <v>0</v>
       </c>
       <c r="AR137" s="5">
-        <v>0</v>
+        <v>121599.99999999997</v>
       </c>
       <c r="AS137" s="5">
-        <v>0</v>
+        <v>243199.99999999997</v>
       </c>
       <c r="AT137" s="5">
-        <v>0</v>
+        <v>364799.99999999994</v>
       </c>
       <c r="AU137" s="5">
-        <v>0</v>
+        <v>486400</v>
       </c>
       <c r="AV137" s="5">
-        <v>0</v>
+        <v>608000</v>
       </c>
       <c r="AW137" s="5">
-        <v>0</v>
+        <v>729600</v>
       </c>
       <c r="AX137" s="5">
-        <v>0</v>
+        <v>851200</v>
       </c>
       <c r="AY137" s="5">
-        <v>0</v>
+        <v>972800.00000000012</v>
       </c>
       <c r="AZ137" s="5">
-        <v>0</v>
+        <v>1094400</v>
       </c>
       <c r="BA137" s="5">
-        <v>0</v>
+        <v>1216000</v>
       </c>
       <c r="BB137" s="5">
-        <v>0</v>
+        <v>1391000</v>
       </c>
       <c r="BC137" s="5">
-        <v>0</v>
+        <v>1566000</v>
       </c>
       <c r="BD137" s="5">
-        <v>0</v>
+        <v>1741000</v>
       </c>
       <c r="BE137" s="5">
-        <v>0</v>
+        <v>1916000</v>
       </c>
       <c r="BF137" s="5">
-        <v>0</v>
+        <v>2091000</v>
       </c>
       <c r="BG137" s="5">
-        <v>0</v>
+        <v>2338000</v>
       </c>
       <c r="BH137" s="5">
-        <v>0</v>
+        <v>2585000</v>
       </c>
       <c r="BI137" s="5">
-        <v>0</v>
+        <v>2832000</v>
       </c>
       <c r="BJ137" s="5">
-        <v>0</v>
+        <v>2358000</v>
       </c>
       <c r="BK137" s="5">
-        <v>0</v>
+        <v>2857000</v>
       </c>
       <c r="BL137" s="5">
-        <v>0</v>
+        <v>3032000</v>
       </c>
       <c r="BM137" s="5">
-        <v>0</v>
+        <v>3239000</v>
       </c>
       <c r="BN137" s="5">
-        <v>0</v>
+        <v>3344666.666666667</v>
       </c>
       <c r="BO137" s="5">
-        <v>0</v>
+        <v>3450333.3333333335</v>
       </c>
       <c r="BP137" s="5">
-        <v>0</v>
+        <v>3556000</v>
       </c>
       <c r="BQ137" s="5">
-        <v>0</v>
+        <v>3817500</v>
       </c>
       <c r="BR137" s="5">
-        <v>0</v>
+        <v>4079000</v>
       </c>
       <c r="BS137" s="5">
-        <v>0</v>
+        <v>4149000</v>
       </c>
       <c r="BT137" s="5">
-        <v>0</v>
+        <v>3870000</v>
       </c>
       <c r="BU137" s="5">
-        <v>0</v>
+        <v>4114000</v>
       </c>
       <c r="BV137" s="5">
-        <v>3822000</v>
+        <v>4696000</v>
       </c>
       <c r="BW137" s="5">
-        <v>0</v>
+        <v>3544000</v>
       </c>
       <c r="BX137" s="5">
-        <v>0</v>
+        <v>4756000</v>
       </c>
       <c r="BY137" s="5">
-        <v>0</v>
+        <v>5149000</v>
       </c>
       <c r="BZ137" s="5">
-        <v>0</v>
+        <v>5214000</v>
       </c>
       <c r="CA137" s="5">
-        <v>0</v>
+        <v>5588000</v>
       </c>
       <c r="CB137" s="5">
-        <v>0</v>
+        <v>6092000</v>
       </c>
       <c r="CC137" s="5">
-        <v>0</v>
+        <v>5957000</v>
       </c>
       <c r="CD137" s="5">
-        <v>0</v>
+        <v>6232000</v>
       </c>
       <c r="CE137" s="5">
-        <v>0</v>
+        <v>6690000</v>
       </c>
       <c r="CF137" s="5">
-        <v>4630000</v>
+        <v>6412000</v>
       </c>
       <c r="CG137" s="5">
-        <v>0</v>
+        <v>5952000</v>
       </c>
       <c r="CH137" s="5">
-        <v>0</v>
+        <v>5162169.179012063</v>
       </c>
       <c r="CI137" s="5">
-        <v>0</v>
+        <v>6063755.7142684031</v>
       </c>
       <c r="CJ137" s="5">
-        <v>0</v>
+        <v>5986868.9773553461</v>
       </c>
       <c r="CK137" s="5">
-        <v>0</v>
+        <v>6523078.0131333433</v>
       </c>
       <c r="CL137" s="5">
-        <v>0</v>
+        <v>7540636.5455668215</v>
       </c>
       <c r="CM137" s="5">
-        <v>0</v>
+        <v>8327120.7769263657</v>
       </c>
       <c r="CN137" s="5">
-        <v>0</v>
+        <v>7181131.1996327285</v>
       </c>
       <c r="CO137" s="5">
-        <v>0</v>
+        <v>8444639.6759754959</v>
       </c>
       <c r="CP137" s="5">
-        <v>8961000</v>
+        <v>9167826.7030393016</v>
       </c>
       <c r="CQ137" s="5">
-        <v>0</v>
+        <v>10518314.691625198</v>
       </c>
       <c r="CR137" s="5">
-        <v>0</v>
+        <v>10857187.023997378</v>
       </c>
       <c r="CS137" s="5">
-        <v>0</v>
+        <v>9899218.7394929305</v>
       </c>
       <c r="CT137" s="5">
-        <v>0</v>
+        <v>10088668.660818744</v>
       </c>
       <c r="CU137" s="5">
-        <v>0</v>
+        <v>10774792.301445104</v>
       </c>
       <c r="CV137" s="5">
-        <v>0</v>
+        <v>11235602.768337155</v>
       </c>
       <c r="CW137" s="5">
-        <v>0</v>
+        <v>12751710.752013853</v>
       </c>
       <c r="CX137" s="5">
-        <v>0</v>
+        <v>13396950.563367529</v>
       </c>
       <c r="CY137" s="5">
-        <v>0</v>
+        <v>12320414.754959952</v>
       </c>
       <c r="CZ137" s="5">
-        <v>14849000</v>
+        <v>15142463.690463001</v>
       </c>
       <c r="DA137" s="5">
-        <v>0</v>
+        <v>16393068.430813657</v>
       </c>
       <c r="DB137" s="5">
-        <v>0</v>
+        <v>15859474.648426574</v>
       </c>
       <c r="DC137" s="5">
-        <v>0</v>
+        <v>16899474.512925733</v>
       </c>
       <c r="DD137" s="5">
-        <v>0</v>
+        <v>17103629.600499108</v>
       </c>
       <c r="DE137" s="5">
-        <v>20740000</v>
+        <v>19036294.908140875</v>
       </c>
       <c r="DF137" s="5">
-        <v>0</v>
+        <v>20264541.696850184</v>
       </c>
       <c r="DG137" s="5">
-        <v>0</v>
+        <v>19568931.0502716</v>
       </c>
       <c r="DH137" s="5">
-        <v>0</v>
+        <v>19513066.052910913</v>
       </c>
       <c r="DI137" s="5">
-        <v>0</v>
+        <v>21672738.875005379</v>
       </c>
       <c r="DJ137" s="5">
-        <v>25316000</v>
+        <v>21836385.217074171</v>
       </c>
       <c r="DK137" s="5">
         <v>22759300</v>
@@ -66485,8 +68115,20 @@
       <c r="FE137" s="5">
         <v>52277015</v>
       </c>
+      <c r="FG137" s="10">
+        <f t="shared" si="8"/>
+        <v>2.4052880647168085E-2</v>
+      </c>
+      <c r="FH137" s="10">
+        <f t="shared" si="6"/>
+        <v>5.2428708930419579E-2</v>
+      </c>
+      <c r="FI137" s="10">
+        <f t="shared" si="7"/>
+        <v>8.1202248396190752E-2</v>
+      </c>
     </row>
-    <row r="138" spans="1:161">
+    <row r="138" spans="1:165">
       <c r="A138" t="s">
         <v>138</v>
       </c>
@@ -66970,8 +68612,20 @@
       <c r="FE138" s="5">
         <v>0</v>
       </c>
+      <c r="FG138" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="FH138" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="FI138" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
     </row>
-    <row r="139" spans="1:161">
+    <row r="139" spans="1:165">
       <c r="A139" t="s">
         <v>139</v>
       </c>
@@ -67455,8 +69109,20 @@
       <c r="FE139" s="5">
         <v>73000</v>
       </c>
+      <c r="FG139" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="FH139" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="FI139" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
     </row>
-    <row r="140" spans="1:161">
+    <row r="140" spans="1:165">
       <c r="A140" t="s">
         <v>140</v>
       </c>
@@ -67940,8 +69606,20 @@
       <c r="FE140" s="5">
         <v>316000</v>
       </c>
+      <c r="FG140" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="FH140" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="FI140" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
     </row>
-    <row r="141" spans="1:161">
+    <row r="141" spans="1:165">
       <c r="A141" t="s">
         <v>141</v>
       </c>
@@ -68425,8 +70103,20 @@
       <c r="FE141" s="5">
         <v>0</v>
       </c>
+      <c r="FG141" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="FH141" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="FI141" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
     </row>
-    <row r="142" spans="1:161">
+    <row r="142" spans="1:165">
       <c r="A142" t="s">
         <v>142</v>
       </c>
@@ -68910,8 +70600,20 @@
       <c r="FE142" s="5">
         <v>0</v>
       </c>
+      <c r="FG142" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="FH142" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="FI142" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
     </row>
-    <row r="143" spans="1:161">
+    <row r="143" spans="1:165">
       <c r="A143" s="6" t="s">
         <v>143</v>
       </c>
@@ -69395,8 +71097,20 @@
       <c r="FE143" s="5">
         <v>47000</v>
       </c>
+      <c r="FG143" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="FH143" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="FI143" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
     </row>
-    <row r="144" spans="1:161">
+    <row r="144" spans="1:165">
       <c r="A144" t="s">
         <v>144</v>
       </c>
@@ -69655,13 +71369,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H145:J145 F147 L147:M148 H147:J378 D148:F378 F145 D145:E147 D144:FC144 D4:FE143">
-    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>